<commit_message>
change diagrams created per scenario + transition
</commit_message>
<xml_diff>
--- a/objectmodeldefinition.xlsx
+++ b/objectmodeldefinition.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/stuff/objectmodeldiagramgenerator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46B95A7-A239-3C4D-B926-918D21C07E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72CEBEA-5C28-C245-82B1-6C703C127F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{EA4244F2-FE33-7643-A566-43DD5B4E5092}"/>
   </bookViews>
   <sheets>
     <sheet name="transitionstates" sheetId="19" r:id="rId1"/>
-    <sheet name="scenarios" sheetId="18" r:id="rId2"/>
+    <sheet name="scenarios" sheetId="22" r:id="rId2"/>
     <sheet name="businessevents" sheetId="1" r:id="rId3"/>
     <sheet name="oms_Kupfer_state1" sheetId="2" r:id="rId4"/>
     <sheet name="oms_Kupfer_state2" sheetId="8" r:id="rId5"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18962" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18966" uniqueCount="481">
   <si>
     <t>bevt0001</t>
   </si>
@@ -1539,6 +1539,18 @@
   <si>
     <t>Target state once we have implemented OnePAM Alignment.</t>
   </si>
+  <si>
+    <t>MleJodler</t>
+  </si>
+  <si>
+    <t>Martin creates some objects which refer to data in a different sheet and scenario</t>
+  </si>
+  <si>
+    <t>Just a test.</t>
+  </si>
+  <si>
+    <t>mevt0101</t>
+  </si>
 </sst>
 </file>
 
@@ -1637,7 +1649,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1901,12 +1913,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2098,31 +2123,15 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="65">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -2799,6 +2808,25 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -3289,20 +3317,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{146E6FAE-5442-4148-B80A-2AE103296F59}" name="Table3" displayName="Table3" ref="A1:C16" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5159AD54-BF1D-D441-A45C-D65DA1CD0986}" name="Table36" displayName="Table36" ref="A1:C16" totalsRowShown="0">
   <autoFilter ref="A1:C16" xr:uid="{C0682A79-088A-6444-B944-088363065AF9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6776E720-FE66-4844-AC38-BD2B4F4FAFDE}" name="Key"/>
-    <tableColumn id="2" xr3:uid="{2A705AD5-40F2-D04F-B082-89A54DD6A28D}" name="PredecessorKeys"/>
-    <tableColumn id="3" xr3:uid="{F33D7D8A-0FD8-5144-BF8B-087065860438}" name="Description"/>
+    <tableColumn id="1" xr3:uid="{16B28E7B-04EE-454F-B84C-48849BB5EB18}" name="Key"/>
+    <tableColumn id="2" xr3:uid="{0CA1CD4D-CC6D-AA46-8083-165CA3A6DEE4}" name="PredecessorKeys"/>
+    <tableColumn id="3" xr3:uid="{ACE976C0-1958-EC48-A565-E2EF6F1094C0}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{422A6A28-4F84-CA4D-BC76-24F29CBA51D2}" name="Tabelle1" displayName="Tabelle1" ref="A1:D59" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
-  <autoFilter ref="A1:D59" xr:uid="{422A6A28-4F84-CA4D-BC76-24F29CBA51D2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{422A6A28-4F84-CA4D-BC76-24F29CBA51D2}" name="Tabelle1" displayName="Tabelle1" ref="A1:D62" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+  <autoFilter ref="A1:D62" xr:uid="{422A6A28-4F84-CA4D-BC76-24F29CBA51D2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E843E1F4-E64E-684F-A053-BC1EBA87FC3D}" name="Key" dataDxfId="62"/>
     <tableColumn id="2" xr3:uid="{AD27EB56-E6EA-1B48-8FF5-F0DBDD95396F}" name="Description" dataDxfId="61"/>
@@ -3314,12 +3342,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4839BD3-5D73-734A-B902-529B029081C5}" name="Tabelle2" displayName="Tabelle2" ref="A1:C17" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4839BD3-5D73-734A-B902-529B029081C5}" name="Tabelle2" displayName="Tabelle2" ref="A1:C17" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A1:C17" xr:uid="{C4839BD3-5D73-734A-B902-529B029081C5}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CD4C934D-C638-6641-9429-0635496C9CA8}" name="Convention" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{49EAB0E3-F001-BB4E-9093-217E47E4FDA4}" name="Description" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{2C6C41A4-B550-2949-BD2B-0FF7B652198B}" name="Reasoning" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{CD4C934D-C638-6641-9429-0635496C9CA8}" name="Convention" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{49EAB0E3-F001-BB4E-9093-217E47E4FDA4}" name="Description" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{2C6C41A4-B550-2949-BD2B-0FF7B652198B}" name="Reasoning" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7663,72 +7691,72 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="K6 A4:XFD4 AA6:XFD6 K5:XFD5 A5:J6 A7:XFD10 AI11 A11:AG11 AL11:XFD11 AI18 AL18:XFD18 A18:AG18 A12:XFD17 A19:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="38" priority="15" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="33" priority="15" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6 B4:XFD4 AA6:XFD6 K5:XFD5 B5:J6 B7:XFD10 AI11 B11:AG11 AL11:XFD11 AI18 AL18:XFD18 B18:AG18 B12:XFD17 B19:XFD1048576">
-    <cfRule type="cellIs" dxfId="37" priority="16" operator="notEqual">
+    <cfRule type="cellIs" dxfId="32" priority="16" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG13:AN13">
-    <cfRule type="containsBlanks" dxfId="36" priority="13" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="31" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(AG13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG13:AN13">
-    <cfRule type="cellIs" dxfId="35" priority="14" operator="notEqual">
+    <cfRule type="cellIs" dxfId="30" priority="14" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH11">
-    <cfRule type="containsBlanks" dxfId="34" priority="9" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="29" priority="9" stopIfTrue="1">
       <formula>LEN(TRIM(AH11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH11">
-    <cfRule type="cellIs" dxfId="33" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="10" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ11">
-    <cfRule type="containsBlanks" dxfId="32" priority="7" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="27" priority="7" stopIfTrue="1">
       <formula>LEN(TRIM(AJ11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ11">
-    <cfRule type="cellIs" dxfId="31" priority="8" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="8" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH18">
-    <cfRule type="containsBlanks" dxfId="30" priority="5" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="25" priority="5" stopIfTrue="1">
       <formula>LEN(TRIM(AH18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH18">
-    <cfRule type="cellIs" dxfId="29" priority="6" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ18">
-    <cfRule type="containsBlanks" dxfId="28" priority="3" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="23" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(AJ18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ18">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG20:AN20">
-    <cfRule type="containsBlanks" dxfId="26" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="21" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(AG20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG20:AN20">
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11713,72 +11741,72 @@
     <mergeCell ref="AA2:AF2"/>
   </mergeCells>
   <conditionalFormatting sqref="K6 A4:XFD4 AA6:XFD6 K5:XFD5 A5:J6 A7:XFD10 AI11 A11:AG11 AL11:XFD11 AI18 AL18:XFD18 A18:AG18 A12:XFD17 A19:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="24" priority="13" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="19" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6 B4:XFD4 AA6:XFD6 K5:XFD5 B5:J6 B7:XFD10 AI11 B11:AG11 AL11:XFD11 AI18 AL18:XFD18 B18:AG18 B12:XFD17 B19:XFD1048576">
-    <cfRule type="cellIs" dxfId="23" priority="14" operator="notEqual">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG13:AN13">
-    <cfRule type="containsBlanks" dxfId="22" priority="11" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="17" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(AG13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG13:AN13">
-    <cfRule type="cellIs" dxfId="21" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH11">
-    <cfRule type="containsBlanks" dxfId="20" priority="9" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="15" priority="9" stopIfTrue="1">
       <formula>LEN(TRIM(AH11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH11">
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ11">
-    <cfRule type="containsBlanks" dxfId="18" priority="7" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="13" priority="7" stopIfTrue="1">
       <formula>LEN(TRIM(AJ11))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ11">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH18">
-    <cfRule type="containsBlanks" dxfId="16" priority="5" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="11" priority="5" stopIfTrue="1">
       <formula>LEN(TRIM(AH18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH18">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ18">
-    <cfRule type="containsBlanks" dxfId="14" priority="3" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="9" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(AJ18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ18">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG20:AN20">
-    <cfRule type="containsBlanks" dxfId="12" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="7" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(AG20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG20:AN20">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15863,12 +15891,12 @@
     <mergeCell ref="AA2:AF2"/>
   </mergeCells>
   <conditionalFormatting sqref="K6 A4:XFD4 AA6:XFD6 K5:XFD5 A5:J6 A7:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="10" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6 B4:XFD4 AA6:XFD6 K5:XFD5 B5:J6 B7:XFD1048576">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19952,12 +19980,12 @@
     <mergeCell ref="AA2:AF2"/>
   </mergeCells>
   <conditionalFormatting sqref="K6 A4:XFD4 AA6:XFD6 K5:XFD5 A5:J6 A7:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6 B4:XFD4 AA6:XFD6 K5:XFD5 B5:J6 B7:XFD1048576">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24038,12 +24066,12 @@
     <mergeCell ref="AA2:AF2"/>
   </mergeCells>
   <conditionalFormatting sqref="K6 A4:XFD4 AA6:XFD6 K5:XFD5 A5:J6 A7:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6 B4:XFD4 AA6:XFD6 K5:XFD5 B5:J6 B7:XFD1048576">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24648,11 +24676,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC60F03-B787-8248-9395-1B994E21141A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751DC78E-EA1F-F444-AA26-59A357346CDF}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24848,11 +24876,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A31B61-90E3-1849-BB99-1A270DFBF588}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25529,6 +25557,32 @@
       </c>
       <c r="C59" s="28"/>
       <c r="D59" s="28"/>
+    </row>
+    <row r="60" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A60" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="B60" s="48" t="s">
+        <v>478</v>
+      </c>
+      <c r="C60" s="28" t="s">
+        <v>477</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="22"/>
+      <c r="B61" s="65"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="22"/>
+      <c r="B62" s="65"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -25544,10 +25598,10 @@
   <dimension ref="A1:BB81"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38689,22 +38743,22 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="V53:Z55 AO53:XFD55 AA53:AN57 V56:XFD56 AT60:BB61 BC58:XFD64 AX62:BB63 AT62:AW64 AT65:XFD65 BC66:XFD71 AX65:BB67 K72:XFD81 K66:AW67 K60:AS65 K58:BB59 K57:XFD57 V49:XFD50 K48:XFD48 K5:K6 K7:XFD11 K49:P49 K52:P56 A48:J49 K68:BB68 A5:J11 A51:J68 A70:J81 AA6:XFD6 L4:XFD5 V52:XFD52 K51:XFD51 K70:BB71 A4:K4 A50:P50 A69:BB69 A82:XFD1048576 A12:XFD47">
-    <cfRule type="containsBlanks" dxfId="58" priority="3" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="53" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V53:Z55 AO53:XFD55 AA53:AN57 V56:XFD56 AT60:BB61 BC58:XFD64 AX62:BB63 AT62:AW64 AT65:XFD65 BC66:XFD71 AX65:BB67 B82:XFD1048576 K72:XFD81 K66:AW67 K60:AS65 K58:BB59 K57:XFD57 V49:XFD50 K48:XFD48 K5:K6 K7:XFD11 K49:P49 K52:P56 B48:J49 K68:BB68 B5:J11 B51:J68 B70:J81 AA6:XFD6 L4:XFD5 V52:XFD52 K51:XFD51 K70:BB71 B4:K4 B12:XFD47 B50:P50 B69:BB69">
-    <cfRule type="cellIs" dxfId="57" priority="5" operator="notEqual">
+    <cfRule type="cellIs" dxfId="52" priority="5" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX64:BB64">
-    <cfRule type="containsBlanks" dxfId="56" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="51" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(AX64))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX64:BB64">
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38729,10 +38783,10 @@
   <dimension ref="A1:BB73"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -50562,12 +50616,12 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="V50:Z50 K52:BB53 K51:Z51 K6 K45:XFD45 AT54:BB56 AT57:XFD57 A4:XFD4 AA6:XFD6 K5:XFD5 A5:J6 K46:P46 A45:J46 A47:P47 K48:P50 BC52:XFD56 K54:AS57 A7:XFD44 V46:XFD49 AA50:XFD51 K58:XFD60 A48:J60 A61:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="54" priority="3" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="49" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V50:Z50 K52:BB53 K51:Z51 K6 K45:XFD45 AT54:BB56 AT57:XFD57 B4:XFD4 AA6:XFD6 K5:XFD5 B5:J6 K46:P46 B45:J46 B47:P47 K48:P50 BC52:XFD56 K54:AS57 B7:XFD44 V46:XFD49 AA50:XFD51 K58:XFD60 B48:J60 B61:XFD1048576">
-    <cfRule type="cellIs" dxfId="53" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="48" priority="4" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -54717,12 +54771,12 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="K6 A4:XFD4 AA6:XFD6 K5:XFD5 A5:J6 A7:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="52" priority="3" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="47" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6 B4:XFD4 AA6:XFD6 K5:XFD5 B5:J6 B7:XFD1048576">
-    <cfRule type="cellIs" dxfId="51" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="46" priority="4" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -58708,22 +58762,22 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A14:AG15 AO14:XFD15 A16:XFD1048576 A5:K6 A4:XFD4 AA6:XFD6 L5:XFD5 A7:XFD13">
-    <cfRule type="containsBlanks" dxfId="50" priority="3" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="45" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:AG15 AO14:XFD15 B16:XFD1048576 B5:K6 B4:XFD4 AA6:XFD6 L5:XFD5 B7:XFD13">
-    <cfRule type="cellIs" dxfId="49" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH14:AN15">
-    <cfRule type="containsBlanks" dxfId="48" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="43" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(AH14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH14:AN15">
-    <cfRule type="cellIs" dxfId="47" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -61233,22 +61287,22 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="K6 A4:XFD4 AA6:XFD6 K5:XFD5 A5:J6 A7:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="46" priority="3" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="41" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6 B4:XFD4 AA6:XFD6 K5:XFD5 B5:J6 B7:XFD1048576">
-    <cfRule type="cellIs" dxfId="45" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG12:AN12">
-    <cfRule type="containsBlanks" dxfId="44" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="39" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(AG12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG12:AN12">
-    <cfRule type="cellIs" dxfId="43" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -61273,7 +61327,7 @@
   <dimension ref="A1:BB16"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AN4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="AU15" sqref="AU15"/>
@@ -63757,22 +63811,22 @@
     <mergeCell ref="AA2:AF2"/>
   </mergeCells>
   <conditionalFormatting sqref="K6 A4:XFD4 AA6:XFD6 K5:XFD5 A5:J6 A7:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="42" priority="3" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="37" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6 B4:XFD4 AA6:XFD6 K5:XFD5 B5:J6 B7:XFD1048576">
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG12:AN12">
-    <cfRule type="containsBlanks" dxfId="40" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="35" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(AG12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG12:AN12">
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="notEqual">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -63803,12 +63857,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010077FCAD843BF44A4BABBF8E8FD9F5DAA3" ma:contentTypeVersion="6" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="c6015d074abc3fd8e64f9ef5e21f7cdc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fe6e65e6-3f48-4872-a1e7-e48555659f5f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="02d2ef7fa4d856fff055a3790f8a6335" ns2:_="">
     <xsd:import namespace="fe6e65e6-3f48-4872-a1e7-e48555659f5f"/>
@@ -63966,6 +64014,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44EA3924-C60D-4AB3-8333-F249729C0DDD}">
   <ds:schemaRefs>
@@ -63975,22 +64029,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2124C44-2049-4194-ADAF-B2DF55B36692}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="fe6e65e6-3f48-4872-a1e7-e48555659f5f"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548EC3FD-DB51-454E-B2A6-D1DD66121FF3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -64006,4 +64044,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2124C44-2049-4194-ADAF-B2DF55B36692}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="fe6e65e6-3f48-4872-a1e7-e48555659f5f"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>